<commit_message>
Update reference file after allowing 8:9 range.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/FormulasWithEvaluation.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/FormulasWithEvaluation.xlsx
@@ -578,13 +578,15 @@
       </x:c>
     </x:row>
     <x:row r="13" spans="1:7">
-      <x:c r="A13" s="0">
+      <x:c r="A13" s="0" t="str">
         <x:f>SUM(8:9)</x:f>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:7">
-      <x:c r="A14" s="0">
+      <x:c r="A14" s="0" t="str">
         <x:f>SUM(8:9)</x:f>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>